<commit_message>
fix error str 46 is bad name
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
@@ -483,7 +483,36 @@
         <v/>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="3"/>
+    <row r="3" ht="12.8" customHeight="1" s="3">
+      <c r="A3" t="n">
+        <v>2890</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>чайник маме</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>693</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>глобус</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>подписка тинькоф и яндекс</t>
+        </is>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>